<commit_message>
fine tune and event essential demo
</commit_message>
<xml_diff>
--- a/zssessentials/src/main/webapp/WEB-INF/books/sample.xlsx
+++ b/zssessentials/src/main/webapp/WEB-INF/books/sample.xlsx
@@ -4,26 +4,26 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="345" windowWidth="17460" windowHeight="9465" tabRatio="781" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="345" windowWidth="17460" windowHeight="9465" tabRatio="781" firstSheet="3" activeTab="13"/>
   </bookViews>
   <sheets>
-    <sheet name="HyperLink" sheetId="14" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
-    <sheet name="Protected (1111)" sheetId="2" r:id="rId3"/>
-    <sheet name="UnProtected" sheetId="3" r:id="rId4"/>
-    <sheet name="merge&amp;unMerge" sheetId="4" r:id="rId5"/>
-    <sheet name="AutoFilter" sheetId="5" r:id="rId6"/>
-    <sheet name="AutoFilter Off" sheetId="8" r:id="rId7"/>
-    <sheet name="Chart" sheetId="6" r:id="rId8"/>
-    <sheet name="Chart Inside" sheetId="13" r:id="rId9"/>
-    <sheet name="CellValue" sheetId="7" r:id="rId10"/>
-    <sheet name="Image" sheetId="12" r:id="rId11"/>
-    <sheet name="AutoFill" sheetId="9" r:id="rId12"/>
-    <sheet name="Validation" sheetId="10" r:id="rId13"/>
-    <sheet name="Validation NPE" sheetId="11" r:id="rId14"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Protected (1111)" sheetId="2" r:id="rId2"/>
+    <sheet name="UnProtected" sheetId="3" r:id="rId3"/>
+    <sheet name="merge&amp;unMerge" sheetId="4" r:id="rId4"/>
+    <sheet name="AutoFilter" sheetId="5" r:id="rId5"/>
+    <sheet name="AutoFilter Off" sheetId="8" r:id="rId6"/>
+    <sheet name="Chart" sheetId="6" r:id="rId7"/>
+    <sheet name="Chart Inside" sheetId="13" r:id="rId8"/>
+    <sheet name="CellValue" sheetId="7" r:id="rId9"/>
+    <sheet name="Image" sheetId="12" r:id="rId10"/>
+    <sheet name="AutoFill" sheetId="9" r:id="rId11"/>
+    <sheet name="Validation" sheetId="10" r:id="rId12"/>
+    <sheet name="Validation NPE" sheetId="11" r:id="rId13"/>
+    <sheet name="HyperLink" sheetId="14" r:id="rId14"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">AutoFilter!$C$4:$E$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">AutoFilter!$C$4:$E$11</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
@@ -1049,24 +1049,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="42889216"/>
-        <c:axId val="42890752"/>
+        <c:axId val="82046336"/>
+        <c:axId val="90838144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="42889216"/>
+        <c:axId val="82046336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42890752"/>
+        <c:crossAx val="90838144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="42890752"/>
+        <c:axId val="90838144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1074,7 +1074,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42889216"/>
+        <c:crossAx val="82046336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1086,7 +1086,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1469,24 +1469,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="42925056"/>
-        <c:axId val="41632512"/>
+        <c:axId val="90856064"/>
+        <c:axId val="90874240"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="42925056"/>
+        <c:axId val="90856064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41632512"/>
+        <c:crossAx val="90874240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="41632512"/>
+        <c:axId val="90874240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1494,7 +1494,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42925056"/>
+        <c:crossAx val="90856064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1506,7 +1506,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1905,114 +1905,92 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:C8"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="43.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="8" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3">
-      <c r="B2" s="23" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3">
-      <c r="B3" s="23" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3">
-      <c r="B5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" ht="32.25">
-      <c r="B8" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>65</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
-  <cols>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="e">
-        <f ca="1">XYZ()</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="B1">
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="B2">
+    </row>
+    <row r="4" spans="1:9">
+      <c r="B4" s="5">
+        <v>123</v>
+      </c>
+      <c r="C4" s="6">
+        <v>456</v>
+      </c>
+      <c r="D4">
+        <f>SUM(B4:C4)</f>
+        <v>579</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="B5" s="3">
+        <v>41375</v>
+      </c>
+      <c r="C5" s="4">
+        <v>41375</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="7" customFormat="1">
+      <c r="G9" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2">
-        <v>99.99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="B3">
+      <c r="H9" s="8"/>
+      <c r="I9" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="H10" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" s="20">
-        <v>123456</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="B5">
-        <f>SUM(B1:B3)</f>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="H13" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="70.5" customHeight="1">
+      <c r="A16" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C5">
-        <f>SUM(C1:C3)</f>
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <f>SUM(D1:D3)</f>
-        <v>123655.99</v>
+    </row>
+    <row r="18" spans="2:4" ht="47.25">
+      <c r="B18" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -2022,7 +2000,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1"/>
   <sheetViews>
@@ -2045,7 +2023,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:K5"/>
   <sheetViews>
@@ -2131,7 +2109,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:K8"/>
   <sheetViews>
@@ -2242,7 +2220,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:I8"/>
   <sheetViews>
@@ -2289,104 +2267,54 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I18"/>
+  <dimension ref="B2:C8"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
-    <col min="7" max="7" width="13" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" style="8" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="B4" s="5">
-        <v>123</v>
-      </c>
-      <c r="C4" s="6">
-        <v>456</v>
-      </c>
-      <c r="D4">
-        <f>SUM(B4:C4)</f>
-        <v>579</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="B5" s="3">
-        <v>41375</v>
-      </c>
-      <c r="C5" s="4">
-        <v>41375</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" s="7" customFormat="1">
-      <c r="G9" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="H9" s="8"/>
-      <c r="I9" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="H10" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="H13" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="70.5" customHeight="1">
-      <c r="A16" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="47.25">
-      <c r="B18" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>14</v>
+    <row r="2" spans="2:3">
+      <c r="B2" s="23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3">
+      <c r="B3" s="23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="32.25">
+      <c r="B8" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C5:E7"/>
   <sheetViews>
@@ -2424,7 +2352,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C2:C4"/>
   <sheetViews>
@@ -2450,11 +2378,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D4:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
@@ -2524,7 +2452,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="1"/>
   <dimension ref="C4:E11"/>
@@ -2632,7 +2560,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C4:E11"/>
   <sheetViews>
@@ -2730,7 +2658,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:F12"/>
   <sheetViews>
@@ -2940,7 +2868,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:F12"/>
   <sheetViews>
@@ -3149,4 +3077,76 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="e">
+        <f ca="1">XYZ()</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2">
+        <v>99.99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="20">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5">
+        <f>SUM(B1:B3)</f>
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <f>SUM(C1:C3)</f>
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <f>SUM(D1:D3)</f>
+        <v>123655.99</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>